<commit_message>
Excel writer is stable now
</commit_message>
<xml_diff>
--- a/data/progresivas.xlsx
+++ b/data/progresivas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\caylloma-archivos\codigo\pruebasCodigo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EA851E-2DF6-47F8-ACFF-5A67AA870EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B63F29-7052-4B05-85E1-BEF88B4153E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{EC1102C6-0EC2-4849-B9A2-EE4B468252A1}"/>
+    <workbookView xWindow="888" yWindow="-108" windowWidth="22260" windowHeight="13176" xr2:uid="{EC1102C6-0EC2-4849-B9A2-EE4B468252A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="30">
   <si>
     <t>alcantarilla de dos ojos</t>
   </si>
@@ -477,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05F3E186-4AAF-4FF0-A1C3-95591625CCED}">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,8 +532,8 @@
         <v>12</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F33" si="0">$A$69-A2</f>
-        <v>11050</v>
+        <f>$A$70-A2</f>
+        <v>11070</v>
       </c>
       <c r="G2">
         <v>68</v>
@@ -559,8 +559,8 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <f t="shared" si="0"/>
-        <v>10870</v>
+        <f t="shared" ref="F3:F66" si="0">$A$70-A3</f>
+        <v>10890</v>
       </c>
       <c r="G3">
         <v>67</v>
@@ -587,7 +587,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>10800</v>
+        <v>10820</v>
       </c>
       <c r="G4">
         <v>66</v>
@@ -614,7 +614,7 @@
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>10550</v>
+        <v>10570</v>
       </c>
       <c r="G5">
         <v>65</v>
@@ -641,7 +641,7 @@
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>10300</v>
+        <v>10320</v>
       </c>
       <c r="G6">
         <v>64</v>
@@ -665,7 +665,7 @@
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>10080</v>
+        <v>10100</v>
       </c>
       <c r="G7">
         <v>63</v>
@@ -692,7 +692,7 @@
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>10050</v>
+        <v>10070</v>
       </c>
       <c r="G8">
         <v>62</v>
@@ -719,7 +719,7 @@
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>9800</v>
+        <v>9820</v>
       </c>
       <c r="G9">
         <v>61</v>
@@ -746,7 +746,7 @@
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>9630</v>
+        <v>9650</v>
       </c>
       <c r="G10">
         <v>60</v>
@@ -773,7 +773,7 @@
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>9550</v>
+        <v>9570</v>
       </c>
       <c r="G11">
         <v>59</v>
@@ -800,7 +800,7 @@
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>9300</v>
+        <v>9320</v>
       </c>
       <c r="G12">
         <v>58</v>
@@ -827,7 +827,7 @@
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>9050</v>
+        <v>9070</v>
       </c>
       <c r="G13">
         <v>57</v>
@@ -854,7 +854,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>8800</v>
+        <v>8820</v>
       </c>
       <c r="G14">
         <v>56</v>
@@ -881,7 +881,7 @@
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>8550</v>
+        <v>8570</v>
       </c>
       <c r="G15">
         <v>55</v>
@@ -908,7 +908,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>8300</v>
+        <v>8320</v>
       </c>
       <c r="G16">
         <v>54</v>
@@ -935,7 +935,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>8230</v>
+        <v>8250</v>
       </c>
       <c r="G17">
         <v>53</v>
@@ -962,7 +962,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>8090</v>
+        <v>8110</v>
       </c>
       <c r="G18">
         <v>52</v>
@@ -989,7 +989,7 @@
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>8050</v>
+        <v>8070</v>
       </c>
       <c r="G19">
         <v>51</v>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>7800</v>
+        <v>7820</v>
       </c>
       <c r="G20">
         <v>50</v>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>7550</v>
+        <v>7570</v>
       </c>
       <c r="G21">
         <v>49</v>
@@ -1070,7 +1070,7 @@
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>7300</v>
+        <v>7320</v>
       </c>
       <c r="G22">
         <v>48</v>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>7130</v>
+        <v>7150</v>
       </c>
       <c r="G23">
         <v>47</v>
@@ -1124,7 +1124,7 @@
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>7050</v>
+        <v>7070</v>
       </c>
       <c r="G24">
         <v>46</v>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
-        <v>7020</v>
+        <v>7040</v>
       </c>
       <c r="G25">
         <v>45</v>
@@ -1178,7 +1178,7 @@
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>6800</v>
+        <v>6820</v>
       </c>
       <c r="G26">
         <v>44</v>
@@ -1205,7 +1205,7 @@
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
-        <v>6550</v>
+        <v>6570</v>
       </c>
       <c r="G27">
         <v>43</v>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
-        <v>6300</v>
+        <v>6320</v>
       </c>
       <c r="G28">
         <v>42</v>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
-        <v>6050</v>
+        <v>6070</v>
       </c>
       <c r="G29">
         <v>41</v>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>6020</v>
+        <v>6040</v>
       </c>
       <c r="G30">
         <v>40</v>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
-        <v>5850</v>
+        <v>5870</v>
       </c>
       <c r="G31">
         <v>39</v>
@@ -1337,7 +1337,7 @@
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>5838</v>
+        <v>5858</v>
       </c>
       <c r="G32">
         <v>38</v>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
-        <v>5800</v>
+        <v>5820</v>
       </c>
       <c r="G33">
         <v>37</v>
@@ -1390,8 +1390,8 @@
         <v>12</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F69" si="1">$A$69-A34</f>
-        <v>5550</v>
+        <f t="shared" si="0"/>
+        <v>5570</v>
       </c>
       <c r="G34">
         <v>36</v>
@@ -1417,8 +1417,8 @@
         <v>12</v>
       </c>
       <c r="F35">
-        <f t="shared" si="1"/>
-        <v>5300</v>
+        <f t="shared" si="0"/>
+        <v>5320</v>
       </c>
       <c r="G35">
         <v>35</v>
@@ -1444,8 +1444,8 @@
         <v>12</v>
       </c>
       <c r="F36">
-        <f t="shared" si="1"/>
-        <v>5050</v>
+        <f t="shared" si="0"/>
+        <v>5070</v>
       </c>
       <c r="G36">
         <v>34</v>
@@ -1471,8 +1471,8 @@
         <v>19</v>
       </c>
       <c r="F37">
-        <f t="shared" si="1"/>
-        <v>5020</v>
+        <f t="shared" si="0"/>
+        <v>5040</v>
       </c>
       <c r="G37">
         <v>33</v>
@@ -1498,8 +1498,8 @@
         <v>2</v>
       </c>
       <c r="F38">
-        <f t="shared" si="1"/>
-        <v>4860</v>
+        <f t="shared" si="0"/>
+        <v>4880</v>
       </c>
       <c r="G38">
         <v>32</v>
@@ -1525,8 +1525,8 @@
         <v>12</v>
       </c>
       <c r="F39">
-        <f t="shared" si="1"/>
-        <v>4800</v>
+        <f t="shared" si="0"/>
+        <v>4820</v>
       </c>
       <c r="G39">
         <v>31</v>
@@ -1552,8 +1552,8 @@
         <v>12</v>
       </c>
       <c r="F40">
-        <f t="shared" si="1"/>
-        <v>4550</v>
+        <f t="shared" si="0"/>
+        <v>4570</v>
       </c>
       <c r="G40">
         <v>30</v>
@@ -1579,8 +1579,8 @@
         <v>12</v>
       </c>
       <c r="F41">
-        <f t="shared" si="1"/>
-        <v>4300</v>
+        <f t="shared" si="0"/>
+        <v>4320</v>
       </c>
       <c r="G41">
         <v>29</v>
@@ -1606,8 +1606,8 @@
         <v>12</v>
       </c>
       <c r="F42">
-        <f t="shared" si="1"/>
-        <v>4050</v>
+        <f t="shared" si="0"/>
+        <v>4070</v>
       </c>
       <c r="G42">
         <v>28</v>
@@ -1633,8 +1633,8 @@
         <v>18</v>
       </c>
       <c r="F43">
-        <f t="shared" si="1"/>
-        <v>4030</v>
+        <f t="shared" si="0"/>
+        <v>4050</v>
       </c>
       <c r="G43">
         <v>27</v>
@@ -1660,8 +1660,8 @@
         <v>12</v>
       </c>
       <c r="F44">
-        <f t="shared" si="1"/>
-        <v>3800</v>
+        <f t="shared" si="0"/>
+        <v>3820</v>
       </c>
       <c r="G44">
         <v>26</v>
@@ -1687,8 +1687,8 @@
         <v>1</v>
       </c>
       <c r="F45">
-        <f t="shared" si="1"/>
-        <v>3600</v>
+        <f t="shared" si="0"/>
+        <v>3620</v>
       </c>
       <c r="G45">
         <v>25</v>
@@ -1714,8 +1714,8 @@
         <v>12</v>
       </c>
       <c r="F46">
-        <f t="shared" si="1"/>
-        <v>3550</v>
+        <f t="shared" si="0"/>
+        <v>3570</v>
       </c>
       <c r="G46">
         <v>24</v>
@@ -1741,8 +1741,8 @@
         <v>12</v>
       </c>
       <c r="F47">
-        <f t="shared" si="1"/>
-        <v>3300</v>
+        <f t="shared" si="0"/>
+        <v>3320</v>
       </c>
       <c r="G47">
         <v>23</v>
@@ -1768,8 +1768,8 @@
         <v>12</v>
       </c>
       <c r="F48">
-        <f t="shared" si="1"/>
-        <v>3050</v>
+        <f t="shared" si="0"/>
+        <v>3070</v>
       </c>
       <c r="G48">
         <v>22</v>
@@ -1795,8 +1795,8 @@
         <v>5</v>
       </c>
       <c r="F49">
-        <f t="shared" si="1"/>
-        <v>3020</v>
+        <f t="shared" si="0"/>
+        <v>3040</v>
       </c>
       <c r="G49">
         <v>21</v>
@@ -1822,8 +1822,8 @@
         <v>12</v>
       </c>
       <c r="F50">
-        <f t="shared" si="1"/>
-        <v>2800</v>
+        <f t="shared" si="0"/>
+        <v>2820</v>
       </c>
       <c r="G50">
         <v>20</v>
@@ -1849,8 +1849,8 @@
         <v>12</v>
       </c>
       <c r="F51">
-        <f t="shared" si="1"/>
-        <v>2550</v>
+        <f t="shared" si="0"/>
+        <v>2570</v>
       </c>
       <c r="G51">
         <v>19</v>
@@ -1876,8 +1876,8 @@
         <v>2</v>
       </c>
       <c r="F52">
-        <f t="shared" si="1"/>
-        <v>2470</v>
+        <f t="shared" si="0"/>
+        <v>2490</v>
       </c>
       <c r="G52">
         <v>18</v>
@@ -1903,8 +1903,8 @@
         <v>12</v>
       </c>
       <c r="F53">
-        <f t="shared" si="1"/>
-        <v>2300</v>
+        <f t="shared" si="0"/>
+        <v>2320</v>
       </c>
       <c r="G53">
         <v>17</v>
@@ -1930,8 +1930,8 @@
         <v>6</v>
       </c>
       <c r="F54">
-        <f t="shared" si="1"/>
-        <v>2080</v>
+        <f t="shared" si="0"/>
+        <v>2100</v>
       </c>
       <c r="G54">
         <v>16</v>
@@ -1957,8 +1957,8 @@
         <v>2</v>
       </c>
       <c r="F55">
-        <f t="shared" si="1"/>
-        <v>2020</v>
+        <f t="shared" si="0"/>
+        <v>2040</v>
       </c>
       <c r="G55">
         <v>15</v>
@@ -1984,8 +1984,8 @@
         <v>7</v>
       </c>
       <c r="F56">
-        <f t="shared" si="1"/>
-        <v>1950</v>
+        <f t="shared" si="0"/>
+        <v>1970</v>
       </c>
       <c r="G56">
         <v>14</v>
@@ -2011,8 +2011,8 @@
         <v>12</v>
       </c>
       <c r="F57">
-        <f t="shared" si="1"/>
-        <v>1800</v>
+        <f t="shared" si="0"/>
+        <v>1820</v>
       </c>
       <c r="G57">
         <v>13</v>
@@ -2038,8 +2038,8 @@
         <v>12</v>
       </c>
       <c r="F58">
-        <f t="shared" si="1"/>
-        <v>1550</v>
+        <f t="shared" si="0"/>
+        <v>1570</v>
       </c>
       <c r="G58">
         <v>12</v>
@@ -2065,8 +2065,8 @@
         <v>12</v>
       </c>
       <c r="F59">
-        <f t="shared" si="1"/>
-        <v>1300</v>
+        <f t="shared" si="0"/>
+        <v>1320</v>
       </c>
       <c r="G59">
         <v>11</v>
@@ -2092,8 +2092,8 @@
         <v>24</v>
       </c>
       <c r="F60">
-        <f t="shared" si="1"/>
-        <v>1050</v>
+        <f t="shared" si="0"/>
+        <v>1070</v>
       </c>
       <c r="G60">
         <v>10</v>
@@ -2119,8 +2119,8 @@
         <v>23</v>
       </c>
       <c r="F61">
-        <f t="shared" si="1"/>
-        <v>1050</v>
+        <f t="shared" si="0"/>
+        <v>1070</v>
       </c>
       <c r="G61">
         <v>9</v>
@@ -2146,8 +2146,8 @@
         <v>8</v>
       </c>
       <c r="F62">
-        <f t="shared" si="1"/>
-        <v>910</v>
+        <f t="shared" si="0"/>
+        <v>930</v>
       </c>
       <c r="G62">
         <v>8</v>
@@ -2173,8 +2173,8 @@
         <v>2</v>
       </c>
       <c r="F63">
-        <f t="shared" si="1"/>
-        <v>870</v>
+        <f t="shared" si="0"/>
+        <v>890</v>
       </c>
       <c r="G63">
         <v>7</v>
@@ -2200,8 +2200,8 @@
         <v>12</v>
       </c>
       <c r="F64">
-        <f t="shared" si="1"/>
-        <v>800</v>
+        <f t="shared" si="0"/>
+        <v>820</v>
       </c>
       <c r="G64">
         <v>6</v>
@@ -2227,8 +2227,8 @@
         <v>12</v>
       </c>
       <c r="F65">
-        <f t="shared" si="1"/>
-        <v>550</v>
+        <f t="shared" si="0"/>
+        <v>570</v>
       </c>
       <c r="G65">
         <v>5</v>
@@ -2254,8 +2254,8 @@
         <v>12</v>
       </c>
       <c r="F66">
-        <f t="shared" si="1"/>
-        <v>300</v>
+        <f t="shared" si="0"/>
+        <v>320</v>
       </c>
       <c r="G66">
         <v>4</v>
@@ -2281,8 +2281,8 @@
         <v>12</v>
       </c>
       <c r="F67">
-        <f t="shared" si="1"/>
-        <v>50</v>
+        <f t="shared" ref="F67:F70" si="1">$A$70-A67</f>
+        <v>70</v>
       </c>
       <c r="G67">
         <v>3</v>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="F68">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G68">
         <v>2</v>
@@ -2336,12 +2336,39 @@
       </c>
       <c r="F69">
         <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>11070</v>
+      </c>
+      <c r="B70" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" t="s">
+        <v>17</v>
+      </c>
+      <c r="E70" t="s">
+        <v>8</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G69">
-        <v>1</v>
-      </c>
-      <c r="H69">
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
         <v>1</v>
       </c>
     </row>

</xml_diff>